<commit_message>
Links for RCMP scraping
</commit_message>
<xml_diff>
--- a/sources/police_jurisdictions/sources.xlsx
+++ b/sources/police_jurisdictions/sources.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Province</t>
   </si>
@@ -34,6 +34,69 @@
   </si>
   <si>
     <t>Special Note</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Police Service</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>https://mern.gouv.qc.ca/territoire/portrait/portrait-donnees-mille.jsp</t>
+  </si>
+  <si>
+    <t>Adminstrative Regions</t>
+  </si>
+  <si>
+    <t>Surêté Québec</t>
+  </si>
+  <si>
+    <t>Counties</t>
+  </si>
+  <si>
+    <t>https://www.ontario.ca/data/municipal-boundaries</t>
+  </si>
+  <si>
+    <t>Ontario Provincial Police</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Shapefile</t>
+  </si>
+  <si>
+    <t>https://data.novascotia.ca/browse?q=Nova%20Scotia%20Topographic%20Database%20-%20County%20Boundaries&amp;sortBy=relevance</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>Detachments</t>
+  </si>
+  <si>
+    <t>RCMP</t>
+  </si>
+  <si>
+    <t>http://www.rcmp-grc.gc.ca/detach/en/d/697/kml</t>
+  </si>
+  <si>
+    <t>KML</t>
+  </si>
+  <si>
+    <t>Needs scraping</t>
   </si>
 </sst>
 </file>
@@ -57,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,12 +128,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,35 +424,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD23"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="159.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>